<commit_message>
Instruction Sb Sw Sh addressing mode changed
</commit_message>
<xml_diff>
--- a/Docs/AHPL/Decodificador Registers.xlsx
+++ b/Docs/AHPL/Decodificador Registers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\RISC-V-Processor-AHPL\Docs\AHPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2207E0-0691-413D-BC3C-3AF7571FBEB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966B5B2B-C57A-44FB-8239-C4042653830D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{965C81D9-F707-4E58-B3D5-80031EEC890C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="56">
   <si>
     <t>Input Addrss</t>
   </si>
@@ -205,13 +205,16 @@
   </si>
   <si>
     <t>use 31 bits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registers(IR_Registers(11 : 7)) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +248,20 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="22">
     <fill>
@@ -274,12 +291,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,6 +384,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -634,99 +651,93 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -738,10 +749,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -753,19 +764,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="21" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="20" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -783,10 +794,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -795,50 +806,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1241,8 +1267,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1264,127 +1290,127 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="70" t="s">
+      <c r="F2" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="63" t="s">
+      <c r="G2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="60" t="s">
+      <c r="H2" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="63" t="s">
+      <c r="I2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="60" t="s">
+      <c r="J2" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="66" t="s">
+      <c r="K2" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="56" t="s">
+      <c r="L2" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="59" t="s">
+      <c r="M2" s="57" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="57"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
+      <c r="A3" s="55"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
     </row>
     <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="57"/>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="40">
+      <c r="A5" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="38">
         <v>0</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="40">
+      <c r="F5" s="38">
         <f>C5</f>
         <v>0</v>
       </c>
-      <c r="G5" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="43" t="s">
+      <c r="G5" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="52" t="str">
+      <c r="L5" s="50" t="str">
         <f>DEC2HEX(2^F5)</f>
         <v>1</v>
       </c>
-      <c r="M5" s="55" t="s">
+      <c r="M5" s="53" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="41">
+      <c r="A6" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="39">
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1393,7 +1419,7 @@
       <c r="E6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="41">
+      <c r="F6" s="39">
         <f t="shared" ref="F6:F31" si="0">C6</f>
         <v>1</v>
       </c>
@@ -1409,25 +1435,25 @@
       <c r="J6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="44">
+      <c r="K6" s="42">
         <v>8</v>
       </c>
-      <c r="L6" s="52" t="str">
+      <c r="L6" s="50" t="str">
         <f t="shared" ref="L6:L31" si="1">DEC2HEX(2^F6)</f>
         <v>2</v>
       </c>
-      <c r="M6" s="55" t="s">
+      <c r="M6" s="53" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="41">
+      <c r="A7" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="39">
         <v>2</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1436,7 +1462,7 @@
       <c r="E7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="41">
+      <c r="F7" s="39">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -1452,25 +1478,25 @@
       <c r="J7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="44" t="s">
+      <c r="K7" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="52" t="str">
+      <c r="L7" s="50" t="str">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="M7" s="55" t="s">
+      <c r="M7" s="53" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="41">
+      <c r="A8" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="39">
         <v>3</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -1479,7 +1505,7 @@
       <c r="E8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="41">
+      <c r="F8" s="39">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1495,25 +1521,25 @@
       <c r="J8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K8" s="44" t="s">
+      <c r="K8" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="L8" s="52" t="str">
+      <c r="L8" s="50" t="str">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="M8" s="55" t="s">
+      <c r="M8" s="53" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="41">
+      <c r="A9" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="39">
         <v>4</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1522,7 +1548,7 @@
       <c r="E9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="41">
+      <c r="F9" s="39">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1538,25 +1564,25 @@
       <c r="J9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K9" s="44" t="s">
+      <c r="K9" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="52" t="str">
+      <c r="L9" s="50" t="str">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="M9" s="55" t="s">
+      <c r="M9" s="53" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="41">
+      <c r="A10" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="39">
         <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -1565,7 +1591,7 @@
       <c r="E10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="41">
+      <c r="F10" s="39">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -1581,17 +1607,17 @@
       <c r="J10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="44">
+      <c r="K10" s="42">
         <v>27</v>
       </c>
-      <c r="L10" s="52" t="str">
+      <c r="L10" s="50" t="str">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="M10" s="55" t="s">
+      <c r="M10" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="N10" s="54" t="s">
+      <c r="N10" s="52" t="s">
         <v>54</v>
       </c>
       <c r="O10">
@@ -1599,13 +1625,13 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="41">
+      <c r="A11" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="39">
         <v>6</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1614,7 +1640,7 @@
       <c r="E11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="41">
+      <c r="F11" s="39">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1630,17 +1656,17 @@
       <c r="J11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="44">
+      <c r="K11" s="42">
         <v>28</v>
       </c>
-      <c r="L11" s="52" t="str">
+      <c r="L11" s="50" t="str">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="M11" s="55" t="s">
+      <c r="M11" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="N11" s="54" t="s">
+      <c r="N11" s="52" t="s">
         <v>54</v>
       </c>
       <c r="O11">
@@ -1648,13 +1674,13 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="41">
+      <c r="A12" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="39">
         <v>7</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -1663,7 +1689,7 @@
       <c r="E12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="41">
+      <c r="F12" s="39">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -1679,17 +1705,17 @@
       <c r="J12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="44" t="s">
+      <c r="K12" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="52" t="str">
+      <c r="L12" s="50" t="str">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="M12" s="52" t="s">
+      <c r="M12" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="N12" s="45" t="s">
+      <c r="N12" s="43" t="s">
         <v>54</v>
       </c>
       <c r="O12">
@@ -1697,13 +1723,13 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="41">
+      <c r="A13" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="39">
         <v>8</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1712,7 +1738,7 @@
       <c r="E13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="41">
+      <c r="F13" s="39">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -1728,17 +1754,17 @@
       <c r="J13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="44">
+      <c r="K13" s="42">
         <v>30</v>
       </c>
-      <c r="L13" s="52" t="str">
+      <c r="L13" s="50" t="str">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="M13" s="52" t="s">
+      <c r="M13" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="N13" s="45" t="s">
+      <c r="N13" s="43" t="s">
         <v>54</v>
       </c>
       <c r="O13">
@@ -1746,13 +1772,13 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="41">
+      <c r="A14" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="39">
         <v>9</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -1761,14 +1787,14 @@
       <c r="E14" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="41">
+      <c r="F14" s="39">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="73" t="s">
         <v>7</v>
       </c>
       <c r="I14" s="19" t="s">
@@ -1777,14 +1803,14 @@
       <c r="J14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K14" s="44">
+      <c r="K14" s="42">
         <v>31</v>
       </c>
-      <c r="L14" s="52" t="str">
+      <c r="L14" s="50" t="str">
         <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="M14" s="52" t="s">
+      <c r="M14" s="50" t="s">
         <v>51</v>
       </c>
       <c r="N14" t="s">
@@ -1795,30 +1821,30 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="41">
+      <c r="A15" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="39">
         <v>10</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="19" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="41">
+      <c r="F15" s="39">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>48</v>
+      <c r="H15" s="72" t="s">
+        <v>55</v>
       </c>
       <c r="I15" s="19" t="s">
         <v>7</v>
@@ -1826,42 +1852,42 @@
       <c r="J15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K15" s="44" t="s">
+      <c r="K15" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="52" t="str">
+      <c r="L15" s="50" t="str">
         <f t="shared" si="1"/>
         <v>400</v>
       </c>
-      <c r="M15" s="52" t="s">
+      <c r="M15" s="50" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="41">
+      <c r="A16" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="39">
         <v>11</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="19" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="41">
+      <c r="F16" s="39">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>48</v>
+      <c r="H16" s="72" t="s">
+        <v>55</v>
       </c>
       <c r="I16" s="19" t="s">
         <v>7</v>
@@ -1869,42 +1895,42 @@
       <c r="J16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="44" t="s">
+      <c r="K16" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="L16" s="52" t="str">
+      <c r="L16" s="50" t="str">
         <f t="shared" si="1"/>
         <v>800</v>
       </c>
-      <c r="M16" s="52" t="s">
+      <c r="M16" s="50" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="41">
+      <c r="A17" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="39">
         <v>12</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="19" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="41">
+      <c r="F17" s="39">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="G17" s="24" t="s">
+      <c r="G17" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>48</v>
+      <c r="H17" s="72" t="s">
+        <v>55</v>
       </c>
       <c r="I17" s="19" t="s">
         <v>7</v>
@@ -1912,25 +1938,25 @@
       <c r="J17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K17" s="44" t="s">
+      <c r="K17" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="L17" s="52" t="str">
+      <c r="L17" s="50" t="str">
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-      <c r="M17" s="52" t="s">
+      <c r="M17" s="50" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="41">
+      <c r="A18" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="39">
         <v>13</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -1939,14 +1965,14 @@
       <c r="E18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="41">
+      <c r="F18" s="39">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H18" s="25" t="s">
+      <c r="H18" s="72" t="s">
         <v>42</v>
       </c>
       <c r="I18" s="19" t="s">
@@ -1955,22 +1981,22 @@
       <c r="J18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K18" s="44" t="s">
+      <c r="K18" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="L18" s="52" t="str">
+      <c r="L18" s="50" t="str">
         <f t="shared" si="1"/>
         <v>2000</v>
       </c>
-      <c r="M18" s="52" t="s">
+      <c r="M18" s="50" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="47" t="s">
+      <c r="A19" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="45" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="1">
@@ -1989,7 +2015,7 @@
       <c r="G19" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="72" t="s">
         <v>42</v>
       </c>
       <c r="I19" s="19" t="s">
@@ -1998,25 +2024,25 @@
       <c r="J19" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K19" s="35">
+      <c r="K19" s="33">
         <v>39</v>
       </c>
-      <c r="L19" s="52" t="str">
+      <c r="L19" s="50" t="str">
         <f t="shared" si="1"/>
         <v>4000</v>
       </c>
-      <c r="M19" s="52" t="s">
+      <c r="M19" s="50" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="41">
+      <c r="A20" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="39">
         <v>15</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -2025,7 +2051,7 @@
       <c r="E20" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="41">
+      <c r="F20" s="39">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -2041,25 +2067,25 @@
       <c r="J20" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K20" s="44">
+      <c r="K20" s="42">
         <v>42</v>
       </c>
-      <c r="L20" s="52" t="str">
+      <c r="L20" s="50" t="str">
         <f t="shared" si="1"/>
         <v>8000</v>
       </c>
-      <c r="M20" s="52" t="s">
+      <c r="M20" s="50" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="41">
+      <c r="A21" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="39">
         <v>16</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -2068,7 +2094,7 @@
       <c r="E21" s="13">
         <v>0</v>
       </c>
-      <c r="F21" s="41">
+      <c r="F21" s="39">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -2084,22 +2110,22 @@
       <c r="J21" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K21" s="44">
+      <c r="K21" s="42">
         <v>43</v>
       </c>
-      <c r="L21" s="52" t="str">
+      <c r="L21" s="50" t="str">
         <f t="shared" si="1"/>
         <v>10000</v>
       </c>
-      <c r="M21" s="52" t="s">
+      <c r="M21" s="50" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="47" t="s">
+      <c r="A22" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="45" t="s">
         <v>41</v>
       </c>
       <c r="C22" s="1">
@@ -2115,7 +2141,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="G22" s="26" t="s">
+      <c r="G22" s="24" t="s">
         <v>9</v>
       </c>
       <c r="H22" s="7" t="s">
@@ -2127,22 +2153,22 @@
       <c r="J22" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K22" s="35" t="s">
+      <c r="K22" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="L22" s="52" t="str">
+      <c r="L22" s="50" t="str">
         <f t="shared" si="1"/>
         <v>20000</v>
       </c>
-      <c r="M22" s="52" t="s">
+      <c r="M22" s="50" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="47" t="s">
+      <c r="A23" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="45" t="s">
         <v>41</v>
       </c>
       <c r="C23" s="1">
@@ -2170,25 +2196,25 @@
       <c r="J23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K23" s="35" t="s">
+      <c r="K23" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="L23" s="52" t="str">
+      <c r="L23" s="50" t="str">
         <f t="shared" si="1"/>
         <v>40000</v>
       </c>
-      <c r="M23" s="52" t="s">
+      <c r="M23" s="50" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="41">
+      <c r="A24" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="39">
         <v>19</v>
       </c>
       <c r="D24" s="3" t="s">
@@ -2197,7 +2223,7 @@
       <c r="E24" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="41">
+      <c r="F24" s="39">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -2213,25 +2239,25 @@
       <c r="J24" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K24" s="44">
+      <c r="K24" s="42">
         <v>67</v>
       </c>
-      <c r="L24" s="52" t="str">
+      <c r="L24" s="50" t="str">
         <f t="shared" si="1"/>
         <v>80000</v>
       </c>
-      <c r="M24" s="52" t="s">
+      <c r="M24" s="50" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="50" t="s">
+      <c r="A25" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="41">
+      <c r="B25" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="39">
         <v>20</v>
       </c>
       <c r="D25" s="5" t="s">
@@ -2240,11 +2266,11 @@
       <c r="E25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="41">
+      <c r="F25" s="39">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G25" s="27" t="s">
+      <c r="G25" s="25" t="s">
         <v>30</v>
       </c>
       <c r="H25" s="7" t="s">
@@ -2256,23 +2282,23 @@
       <c r="J25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K25" s="44">
+      <c r="K25" s="42">
         <v>68</v>
       </c>
-      <c r="L25" s="52" t="str">
+      <c r="L25" s="50" t="str">
         <f t="shared" si="1"/>
         <v>100000</v>
       </c>
-      <c r="M25" s="52"/>
+      <c r="M25" s="50"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="50" t="s">
+      <c r="A26" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="41">
+      <c r="B26" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="39">
         <v>21</v>
       </c>
       <c r="D26" s="5" t="s">
@@ -2281,14 +2307,14 @@
       <c r="E26" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="41">
+      <c r="F26" s="39">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="G26" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="H26" s="25" t="s">
+      <c r="H26" s="23" t="s">
         <v>42</v>
       </c>
       <c r="I26" s="21" t="s">
@@ -2297,23 +2323,23 @@
       <c r="J26" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K26" s="44" t="s">
+      <c r="K26" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="L26" s="52" t="str">
+      <c r="L26" s="50" t="str">
         <f t="shared" si="1"/>
         <v>200000</v>
       </c>
-      <c r="M26" s="52"/>
+      <c r="M26" s="50"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="50" t="s">
+      <c r="A27" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="41">
+      <c r="B27" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="39">
         <v>22</v>
       </c>
       <c r="D27" s="5" t="s">
@@ -2322,11 +2348,11 @@
       <c r="E27" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="41">
+      <c r="F27" s="39">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="G27" s="26" t="s">
+      <c r="G27" s="24" t="s">
         <v>9</v>
       </c>
       <c r="H27" s="12" t="s">
@@ -2338,23 +2364,23 @@
       <c r="J27" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K27" s="44" t="s">
+      <c r="K27" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="L27" s="52" t="str">
+      <c r="L27" s="50" t="str">
         <f t="shared" si="1"/>
         <v>400000</v>
       </c>
-      <c r="M27" s="52"/>
+      <c r="M27" s="50"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" s="41">
+      <c r="B28" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="39">
         <v>23</v>
       </c>
       <c r="D28" s="5" t="s">
@@ -2363,14 +2389,14 @@
       <c r="E28" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="41">
+      <c r="F28" s="39">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="G28" s="24" t="s">
+      <c r="G28" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="28" t="s">
+      <c r="H28" s="26" t="s">
         <v>47</v>
       </c>
       <c r="I28" s="19" t="s">
@@ -2379,23 +2405,23 @@
       <c r="J28" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K28" s="44" t="s">
+      <c r="K28" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="L28" s="52" t="str">
+      <c r="L28" s="50" t="str">
         <f t="shared" si="1"/>
         <v>800000</v>
       </c>
-      <c r="M28" s="52"/>
+      <c r="M28" s="50"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="50" t="s">
+      <c r="A29" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29" s="41">
+      <c r="B29" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="39">
         <v>24</v>
       </c>
       <c r="D29" s="5" t="s">
@@ -2404,11 +2430,11 @@
       <c r="E29" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F29" s="41">
+      <c r="F29" s="39">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="G29" s="29" t="s">
+      <c r="G29" s="27" t="s">
         <v>34</v>
       </c>
       <c r="H29" s="12" t="s">
@@ -2420,23 +2446,23 @@
       <c r="J29" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K29" s="44">
+      <c r="K29" s="42">
         <v>95</v>
       </c>
-      <c r="L29" s="52" t="str">
+      <c r="L29" s="50" t="str">
         <f t="shared" si="1"/>
         <v>1000000</v>
       </c>
-      <c r="M29" s="52"/>
+      <c r="M29" s="50"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="50" t="s">
+      <c r="A30" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="41">
+      <c r="B30" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="39">
         <v>25</v>
       </c>
       <c r="D30" s="5" t="s">
@@ -2445,14 +2471,14 @@
       <c r="E30" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="41">
+      <c r="F30" s="39">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="G30" s="30" t="s">
+      <c r="G30" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="H30" s="31" t="s">
+      <c r="H30" s="29" t="s">
         <v>46</v>
       </c>
       <c r="I30" s="19" t="s">
@@ -2461,23 +2487,23 @@
       <c r="J30" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K30" s="44" t="s">
+      <c r="K30" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="L30" s="52" t="str">
+      <c r="L30" s="50" t="str">
         <f t="shared" si="1"/>
         <v>2000000</v>
       </c>
-      <c r="M30" s="52"/>
+      <c r="M30" s="50"/>
     </row>
     <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="48" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="42">
+      <c r="B31" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="40">
         <v>26</v>
       </c>
       <c r="D31" s="16" t="s">
@@ -2486,30 +2512,30 @@
       <c r="E31" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="42">
+      <c r="F31" s="40">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="G31" s="32" t="s">
+      <c r="G31" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="H31" s="33" t="s">
+      <c r="H31" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="I31" s="34" t="s">
+      <c r="I31" s="32" t="s">
         <v>7</v>
       </c>
       <c r="J31" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="K31" s="42">
+      <c r="K31" s="40">
         <v>58</v>
       </c>
-      <c r="L31" s="53" t="str">
+      <c r="L31" s="51" t="str">
         <f t="shared" si="1"/>
         <v>4000000</v>
       </c>
-      <c r="M31" s="53"/>
+      <c r="M31" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2742,18 +2768,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2775,14 +2801,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB625FBE-2784-45D8-A21C-844EC73CE14E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59816EE9-EA4D-4134-8D63-408F9CD605F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2796,4 +2814,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB625FBE-2784-45D8-A21C-844EC73CE14E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Alu simulation and correction completed
</commit_message>
<xml_diff>
--- a/Docs/AHPL/Decodificador Registers.xlsx
+++ b/Docs/AHPL/Decodificador Registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\RISC-V-Processor-AHPL\Docs\AHPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\GitHub\RISC-V-Processor-AHPL\Docs\AHPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966B5B2B-C57A-44FB-8239-C4042653830D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAFAA11-FF4C-4A58-B67D-9D890BD64C59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{965C81D9-F707-4E58-B3D5-80031EEC890C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{965C81D9-F707-4E58-B3D5-80031EEC890C}"/>
   </bookViews>
   <sheets>
     <sheet name="Decodificador" sheetId="2" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>7 10 59</t>
-  </si>
-  <si>
     <t>Registers_ALU(31:0)</t>
   </si>
   <si>
@@ -208,6 +205,9 @@
   </si>
   <si>
     <t xml:space="preserve">Registers(IR_Registers(11 : 7)) </t>
+  </si>
+  <si>
+    <t>7 10 54 53 59</t>
   </si>
 </sst>
 </file>
@@ -806,6 +806,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -850,21 +865,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1268,110 +1268,110 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.21875" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.28515625" customWidth="1"/>
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="54" t="s">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="59" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="72" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="67" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="68" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="68" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="61" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="58" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="61" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="64" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="M2" s="57" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="55"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-    </row>
-    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="55"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M2" s="62" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="60"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="60"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="38">
         <v>0</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="35" t="s">
         <v>6</v>
@@ -1393,31 +1393,31 @@
         <v>7</v>
       </c>
       <c r="K5" s="41" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="L5" s="50" t="str">
         <f>DEC2HEX(2^F5)</f>
         <v>1</v>
       </c>
       <c r="M5" s="53" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="39">
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="F6" s="39">
         <f t="shared" ref="F6:F31" si="0">C6</f>
@@ -1443,15 +1443,15 @@
         <v>2</v>
       </c>
       <c r="M6" s="53" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="39">
         <v>2</v>
@@ -1467,34 +1467,34 @@
         <v>2</v>
       </c>
       <c r="G7" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="42" t="s">
         <v>9</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7" s="42" t="s">
-        <v>10</v>
       </c>
       <c r="L7" s="50" t="str">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="M7" s="53" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="39">
         <v>3</v>
@@ -1510,34 +1510,34 @@
         <v>3</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I8" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="42" t="s">
         <v>11</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="K8" s="42" t="s">
-        <v>12</v>
       </c>
       <c r="L8" s="50" t="str">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="M8" s="53" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="39">
         <v>4</v>
@@ -1553,43 +1553,43 @@
         <v>4</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K9" s="42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L9" s="50" t="str">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M9" s="53" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="39">
         <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" s="39">
         <f t="shared" si="0"/>
@@ -1615,30 +1615,30 @@
         <v>20</v>
       </c>
       <c r="M10" s="53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N10" s="52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O10">
         <v>6360</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="39">
         <v>6</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="39">
         <f t="shared" si="0"/>
@@ -1664,30 +1664,30 @@
         <v>40</v>
       </c>
       <c r="M11" s="53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N11" s="52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O11">
         <v>8200</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="39">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="39">
-        <v>7</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="E12" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12" s="39">
         <f t="shared" si="0"/>
@@ -1706,37 +1706,37 @@
         <v>7</v>
       </c>
       <c r="K12" s="42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L12" s="50" t="str">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="M12" s="50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N12" s="43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O12">
         <v>9160</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="39">
         <v>8</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F13" s="39">
         <f t="shared" si="0"/>
@@ -1762,30 +1762,30 @@
         <v>100</v>
       </c>
       <c r="M13" s="50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N13" s="43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O13">
         <v>10700</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="39">
         <v>9</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F14" s="39">
         <f t="shared" si="0"/>
@@ -1794,7 +1794,7 @@
       <c r="G14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="73" t="s">
+      <c r="H14" s="58" t="s">
         <v>7</v>
       </c>
       <c r="I14" s="19" t="s">
@@ -1811,21 +1811,21 @@
         <v>200</v>
       </c>
       <c r="M14" s="50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O14">
         <v>11600</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="39">
         <v>10</v>
@@ -1840,35 +1840,35 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G15" s="69" t="s">
+      <c r="G15" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" s="42" t="s">
         <v>20</v>
-      </c>
-      <c r="H15" s="72" t="s">
-        <v>55</v>
-      </c>
-      <c r="I15" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="K15" s="42" t="s">
-        <v>21</v>
       </c>
       <c r="L15" s="50" t="str">
         <f t="shared" si="1"/>
         <v>400</v>
       </c>
       <c r="M15" s="50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="39">
         <v>11</v>
@@ -1883,35 +1883,35 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G16" s="70" t="s">
+      <c r="G16" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="42" t="s">
         <v>22</v>
-      </c>
-      <c r="H16" s="72" t="s">
-        <v>55</v>
-      </c>
-      <c r="I16" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="K16" s="42" t="s">
-        <v>23</v>
       </c>
       <c r="L16" s="50" t="str">
         <f t="shared" si="1"/>
         <v>800</v>
       </c>
       <c r="M16" s="50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="39">
         <v>12</v>
@@ -1926,35 +1926,35 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="G17" s="71" t="s">
+      <c r="G17" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" s="42" t="s">
         <v>24</v>
-      </c>
-      <c r="H17" s="72" t="s">
-        <v>55</v>
-      </c>
-      <c r="I17" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="K17" s="42" t="s">
-        <v>25</v>
       </c>
       <c r="L17" s="50" t="str">
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="M17" s="50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="39">
         <v>13</v>
@@ -1970,10 +1970,10 @@
         <v>13</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="72" t="s">
-        <v>42</v>
+        <v>8</v>
+      </c>
+      <c r="H18" s="57" t="s">
+        <v>41</v>
       </c>
       <c r="I18" s="19" t="s">
         <v>7</v>
@@ -1982,28 +1982,28 @@
         <v>7</v>
       </c>
       <c r="K18" s="42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L18" s="50" t="str">
         <f t="shared" si="1"/>
         <v>2000</v>
       </c>
       <c r="M18" s="50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1">
         <v>14</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>6</v>
@@ -2013,10 +2013,10 @@
         <v>14</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="72" t="s">
-        <v>42</v>
+        <v>8</v>
+      </c>
+      <c r="H19" s="57" t="s">
+        <v>41</v>
       </c>
       <c r="I19" s="19" t="s">
         <v>7</v>
@@ -2032,24 +2032,24 @@
         <v>4000</v>
       </c>
       <c r="M19" s="50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="39">
         <v>15</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F20" s="39">
         <f t="shared" si="0"/>
@@ -2075,21 +2075,21 @@
         <v>8000</v>
       </c>
       <c r="M20" s="50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="39">
         <v>16</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="13">
         <v>0</v>
@@ -2118,21 +2118,21 @@
         <v>10000</v>
       </c>
       <c r="M21" s="50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="1">
         <v>17</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>6</v>
@@ -2142,10 +2142,10 @@
         <v>17</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I22" s="19" t="s">
         <v>7</v>
@@ -2154,28 +2154,28 @@
         <v>7</v>
       </c>
       <c r="K22" s="33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L22" s="50" t="str">
         <f t="shared" si="1"/>
         <v>20000</v>
       </c>
       <c r="M22" s="50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" s="1">
         <v>18</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>6</v>
@@ -2185,43 +2185,43 @@
         <v>18</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I23" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K23" s="33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L23" s="50" t="str">
         <f t="shared" si="1"/>
         <v>40000</v>
       </c>
       <c r="M23" s="50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24" s="39">
         <v>19</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F24" s="39">
         <f t="shared" si="0"/>
@@ -2247,15 +2247,15 @@
         <v>80000</v>
       </c>
       <c r="M24" s="50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="39">
         <v>20</v>
@@ -2271,10 +2271,10 @@
         <v>20</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I25" s="19" t="s">
         <v>7</v>
@@ -2291,12 +2291,12 @@
       </c>
       <c r="M25" s="50"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C26" s="39">
         <v>21</v>
@@ -2312,19 +2312,19 @@
         <v>21</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H26" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I26" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K26" s="42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L26" s="50" t="str">
         <f t="shared" si="1"/>
@@ -2332,12 +2332,12 @@
       </c>
       <c r="M26" s="50"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27" s="39">
         <v>22</v>
@@ -2353,10 +2353,10 @@
         <v>22</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I27" s="19" t="s">
         <v>7</v>
@@ -2365,7 +2365,7 @@
         <v>7</v>
       </c>
       <c r="K27" s="42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L27" s="50" t="str">
         <f t="shared" si="1"/>
@@ -2373,12 +2373,12 @@
       </c>
       <c r="M27" s="50"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C28" s="39">
         <v>23</v>
@@ -2394,10 +2394,10 @@
         <v>23</v>
       </c>
       <c r="G28" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H28" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I28" s="19" t="s">
         <v>7</v>
@@ -2406,7 +2406,7 @@
         <v>7</v>
       </c>
       <c r="K28" s="42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L28" s="50" t="str">
         <f t="shared" si="1"/>
@@ -2414,12 +2414,12 @@
       </c>
       <c r="M28" s="50"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" s="39">
         <v>24</v>
@@ -2435,10 +2435,10 @@
         <v>24</v>
       </c>
       <c r="G29" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I29" s="19" t="s">
         <v>7</v>
@@ -2455,12 +2455,12 @@
       </c>
       <c r="M29" s="50"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" s="39">
         <v>25</v>
@@ -2476,10 +2476,10 @@
         <v>25</v>
       </c>
       <c r="G30" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H30" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I30" s="19" t="s">
         <v>7</v>
@@ -2488,7 +2488,7 @@
         <v>7</v>
       </c>
       <c r="K30" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L30" s="50" t="str">
         <f t="shared" si="1"/>
@@ -2496,12 +2496,12 @@
       </c>
       <c r="M30" s="50"/>
     </row>
-    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="49" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31" s="40">
         <v>26</v>
@@ -2517,10 +2517,10 @@
         <v>26</v>
       </c>
       <c r="G31" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H31" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I31" s="32" t="s">
         <v>7</v>
@@ -2589,13 +2589,16 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="K5" twoDigitTextYear="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100499B73C812517E4B87BCDE641853BAB9" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b68fceede8c5805f76295220e8e44f13">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ad4fc1d6-332d-474d-af02-ccba7dd3642b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="585d2332b120932ddf2a11d4d4e88441" ns2:_="">
     <xsd:import namespace="ad4fc1d6-332d-474d-af02-ccba7dd3642b"/>
@@ -2767,12 +2770,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2783,6 +2780,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59816EE9-EA4D-4134-8D63-408F9CD605F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ad4fc1d6-332d-474d-af02-ccba7dd3642b"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D2CD526-0717-4E70-B506-592509C13EDE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2800,22 +2813,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59816EE9-EA4D-4134-8D63-408F9CD605F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ad4fc1d6-332d-474d-af02-ccba7dd3642b"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB625FBE-2784-45D8-A21C-844EC73CE14E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fixed add registers bug
</commit_message>
<xml_diff>
--- a/Docs/AHPL/Decodificador Registers.xlsx
+++ b/Docs/AHPL/Decodificador Registers.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\RISC-V-Processor-AHPL\Docs\AHPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\GitHub\RISC-V-Processor-AHPL\Docs\AHPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF691ED-815C-405A-AA1F-E2D27CFE2AC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76369D82-0B4C-4FF3-974E-BD45403BC6EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{965C81D9-F707-4E58-B3D5-80031EEC890C}"/>
+    <workbookView xWindow="14040" yWindow="1020" windowWidth="14580" windowHeight="11385" xr2:uid="{965C81D9-F707-4E58-B3D5-80031EEC890C}"/>
   </bookViews>
   <sheets>
     <sheet name="Decodificador" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" iterate="1" iterateCount="1000"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="57">
   <si>
     <t>Input Addrss</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>72 73</t>
+  </si>
+  <si>
+    <t>53 54</t>
   </si>
 </sst>
 </file>
@@ -651,7 +654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -872,11 +875,74 @@
     <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="20" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1271,31 +1337,31 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51099917-B59B-4847-AA5A-0E2A7F2811AB}">
   <sheetPr codeName="Hoja2"/>
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="61" t="s">
         <v>47</v>
       </c>
@@ -1336,7 +1402,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="62"/>
       <c r="B3" s="72"/>
       <c r="C3" s="72"/>
@@ -1351,7 +1417,7 @@
       <c r="L3" s="62"/>
       <c r="M3" s="62"/>
     </row>
-    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="62"/>
       <c r="B4" s="73"/>
       <c r="C4" s="73"/>
@@ -1366,7 +1432,7 @@
       <c r="L4" s="63"/>
       <c r="M4" s="63"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
         <v>39</v>
       </c>
@@ -1409,7 +1475,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
         <v>39</v>
       </c>
@@ -1426,7 +1492,7 @@
         <v>41</v>
       </c>
       <c r="F6" s="39">
-        <f t="shared" ref="F6:F31" si="0">C6</f>
+        <f t="shared" ref="F6:F32" si="0">C6</f>
         <v>1</v>
       </c>
       <c r="G6" s="19" t="s">
@@ -1452,7 +1518,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
         <v>39</v>
       </c>
@@ -1495,7 +1561,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
         <v>39</v>
       </c>
@@ -1538,7 +1604,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
         <v>39</v>
       </c>
@@ -1581,7 +1647,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>39</v>
       </c>
@@ -1630,7 +1696,7 @@
         <v>6360</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="48" t="s">
         <v>39</v>
       </c>
@@ -1679,7 +1745,7 @@
         <v>8200</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
         <v>39</v>
       </c>
@@ -1728,7 +1794,7 @@
         <v>9160</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="48" t="s">
         <v>39</v>
       </c>
@@ -1777,7 +1843,7 @@
         <v>10700</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
         <v>39</v>
       </c>
@@ -1826,7 +1892,7 @@
         <v>11600</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="48" t="s">
         <v>39</v>
       </c>
@@ -1869,7 +1935,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
         <v>39</v>
       </c>
@@ -1912,7 +1978,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
         <v>39</v>
       </c>
@@ -1955,7 +2021,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="48" t="s">
         <v>39</v>
       </c>
@@ -1998,7 +2064,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="48" t="s">
         <v>39</v>
       </c>
@@ -2041,7 +2107,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="48" t="s">
         <v>39</v>
       </c>
@@ -2084,7 +2150,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="48" t="s">
         <v>39</v>
       </c>
@@ -2127,7 +2193,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="48" t="s">
         <v>39</v>
       </c>
@@ -2170,7 +2236,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="s">
         <v>39</v>
       </c>
@@ -2213,7 +2279,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="48" t="s">
         <v>39</v>
       </c>
@@ -2256,7 +2322,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="48" t="s">
         <v>38</v>
       </c>
@@ -2297,7 +2363,7 @@
       </c>
       <c r="M25" s="50"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
         <v>38</v>
       </c>
@@ -2338,7 +2404,7 @@
       </c>
       <c r="M26" s="50"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="48" t="s">
         <v>38</v>
       </c>
@@ -2379,7 +2445,7 @@
       </c>
       <c r="M27" s="50"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="48" t="s">
         <v>38</v>
       </c>
@@ -2420,7 +2486,7 @@
       </c>
       <c r="M28" s="50"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="48" t="s">
         <v>38</v>
       </c>
@@ -2461,7 +2527,7 @@
       </c>
       <c r="M29" s="50"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="48" t="s">
         <v>38</v>
       </c>
@@ -2502,7 +2568,7 @@
       </c>
       <c r="M30" s="50"/>
     </row>
-    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="49" t="s">
         <v>38</v>
       </c>
@@ -2542,6 +2608,42 @@
         <v>4000000</v>
       </c>
       <c r="M31" s="51"/>
+    </row>
+    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="38">
+        <v>27</v>
+      </c>
+      <c r="D32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" s="40">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="G32" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I32" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K32" s="76" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2560,37 +2662,63 @@
     <mergeCell ref="G2:G4"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:B31">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:J31 M5:M11 N10:N11">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+  <conditionalFormatting sqref="D5:J31 M5:M11 N10:N11 F32">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A31">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:L31">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>IF(EXACT(A5,"Y"),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5:M31 N10:N11">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"AllOk"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>"****"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32:E32">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G32:J32">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"****"</formula>
+      <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2774,18 +2902,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2807,6 +2935,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB625FBE-2784-45D8-A21C-844EC73CE14E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59816EE9-EA4D-4134-8D63-408F9CD605F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2820,12 +2956,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB625FBE-2784-45D8-A21C-844EC73CE14E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>